<commit_message>
fix for test failure
</commit_message>
<xml_diff>
--- a/test_resource/codeextractor_F_T.xlsx
+++ b/test_resource/codeextractor_F_T.xlsx
@@ -1,28 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\functiondefextractor\test_resource\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="codeextractor" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Code</t>
   </si>
   <si>
     <t>Uniq ID</t>
-  </si>
-  <si>
-    <t>HelloController.java_Test_AddMethod</t>
   </si>
   <si>
     <t>test.cs_Test_AddMethod</t>
@@ -84,12 +86,18 @@
         }  
 </t>
   </si>
+  <si>
+    <t>TestHelloController.java_Test_AddMethod</t>
+  </si>
+  <si>
+    <t>TstHelloController.java_Test_AddMethod</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +160,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -198,7 +214,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -230,9 +246,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -264,6 +281,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -439,14 +457,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="78.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -454,68 +477,68 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>